<commit_message>
Tilt compensated yaw from mag function added
</commit_message>
<xml_diff>
--- a/analysis/tests_26_12_2020_after_auto_calib.xlsx
+++ b/analysis/tests_26_12_2020_after_auto_calib.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\!Phyton_Source\RPi_car1.0_soft\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F9BF5065-CB36-4017-9808-F3EE81023C94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C68D9B-5F93-47D5-A67A-7860C6178006}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{66404092-53FA-465A-8911-F7C5FBF4D032}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="16">
   <si>
     <t>Motors</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>yaw, deg</t>
+  </si>
+  <si>
+    <t>__yaw</t>
   </si>
 </sst>
 </file>
@@ -1190,6 +1193,446 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11252198031052145"/>
+          <c:y val="0.19721068557655025"/>
+          <c:w val="0.86573884514435695"/>
+          <c:h val="0.77736111111111106"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>__yaw</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$N$2:$N$58</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="57"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-79.949846000000008</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-119.63646866666664</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-137.23505866666665</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-179.25434999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-10.882044666666673</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-14.373535000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-30.372239333333312</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-61.697638666666649</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-77.860047666666617</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-98.694397999999978</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-116.37043699999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-149.0183526666666</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-175.83440000000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-179.46962133333329</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-13.053684000000032</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-34.96407233333332</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-65.23229166666664</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-62.34820133333335</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-117.29189900000006</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-112.7248013333334</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-143.9102166666666</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-174.45932666666658</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-178.45382600000005</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-37.610962666666637</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-33.18410833333337</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-52.248450666666713</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-60.876977333333343</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-112.11438899999996</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-119.75794833333339</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-159.69576833333338</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-157.83128866666664</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-156.43324000000007</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-10.384231333333332</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-21.489542000000029</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-37.978282999999919</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-78.791965333333565</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-75.683770666666646</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-86.477631999999971</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-151.63612933333332</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-2.0269263333333356</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-5.693752666666569</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-45.392747666666651</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-23.403636666666671</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-9.6548303333332797</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>-44.295946000000072</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>-108.63577000000009</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-122.09115399999996</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-160.21116799999982</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-134.28737999999998</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>-30.889729999999872</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>-13.044759999999997</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>-75.724416666666684</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>-40.208918666666705</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>-33.948999000000185</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>-51.951333333333324</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-72F4-4D6D-A317-BFAB43CBE82E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="595501008"/>
+        <c:axId val="595503888"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="595501008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="595503888"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="595503888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="595501008"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1270,6 +1713,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -2276,20 +2759,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>31750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2316,16 +3315,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>168275</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>422275</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>155575</xdr:rowOff>
+      <xdr:rowOff>111125</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>473075</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>117475</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>136525</xdr:rowOff>
+      <xdr:rowOff>92075</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2345,6 +3344,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>421121</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>179822</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>116320</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>160771</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Диаграмма 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82DBAA03-90E7-40A0-A82D-B044122F373D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2650,15 +3685,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31E4F8D0-F519-4A24-AC17-E4BF626A579E}">
-  <dimension ref="A1:M58"/>
+  <dimension ref="A1:N58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="U42" sqref="U42"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="X8" sqref="X8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2698,8 +3733,11 @@
       <c r="M1" t="s">
         <v>14</v>
       </c>
+      <c r="N1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2740,8 +3778,11 @@
         <f>ATAN2(-J2,I2)*180/PI()</f>
         <v>177.06195173024</v>
       </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -2782,8 +3823,12 @@
         <f t="shared" ref="M3:M57" si="0">ATAN2(-J3,I3)*180/PI()</f>
         <v>167.15694103800092</v>
       </c>
+      <c r="N3">
+        <f>MOD((H3*C4+1/6*(0+2*H2+2*H3+H4)), -180)</f>
+        <v>-79.949846000000008</v>
+      </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -2824,8 +3869,12 @@
         <f t="shared" si="0"/>
         <v>130.8480337839876</v>
       </c>
+      <c r="N4">
+        <f t="shared" ref="N4:N57" si="1">MOD((H4*C5+1/6*(0+2*H3+2*H4+H5)), -180)</f>
+        <v>-119.63646866666664</v>
+      </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -2866,8 +3915,12 @@
         <f t="shared" si="0"/>
         <v>106.46049559426666</v>
       </c>
+      <c r="N5">
+        <f t="shared" si="1"/>
+        <v>-137.23505866666665</v>
+      </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -2908,8 +3961,12 @@
         <f t="shared" si="0"/>
         <v>90.479165001522233</v>
       </c>
+      <c r="N6">
+        <f t="shared" si="1"/>
+        <v>-179.25434999999999</v>
+      </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -2950,8 +4007,12 @@
         <f t="shared" si="0"/>
         <v>38.333340109098636</v>
       </c>
+      <c r="N7">
+        <f t="shared" si="1"/>
+        <v>-10.882044666666673</v>
+      </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -2992,8 +4053,12 @@
         <f t="shared" si="0"/>
         <v>-98.464651212373241</v>
       </c>
+      <c r="N8">
+        <f t="shared" si="1"/>
+        <v>-14.373535000000004</v>
+      </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -3034,8 +4099,12 @@
         <f t="shared" si="0"/>
         <v>-108.69730364952055</v>
       </c>
+      <c r="N9">
+        <f t="shared" si="1"/>
+        <v>-30.372239333333312</v>
+      </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -3076,8 +4145,12 @@
         <f t="shared" si="0"/>
         <v>-120.65840400896766</v>
       </c>
+      <c r="N10">
+        <f t="shared" si="1"/>
+        <v>-61.697638666666649</v>
+      </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -3118,8 +4191,12 @@
         <f t="shared" si="0"/>
         <v>-154.11750666021427</v>
       </c>
+      <c r="N11">
+        <f t="shared" si="1"/>
+        <v>-77.860047666666617</v>
+      </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -3160,8 +4237,12 @@
         <f t="shared" si="0"/>
         <v>173.05357891764172</v>
       </c>
+      <c r="N12">
+        <f t="shared" si="1"/>
+        <v>-98.694397999999978</v>
+      </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -3202,8 +4283,12 @@
         <f t="shared" si="0"/>
         <v>145.32481363279933</v>
       </c>
+      <c r="N13">
+        <f t="shared" si="1"/>
+        <v>-116.37043699999998</v>
+      </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -3244,8 +4329,12 @@
         <f t="shared" si="0"/>
         <v>116.25333473279927</v>
       </c>
+      <c r="N14">
+        <f t="shared" si="1"/>
+        <v>-149.0183526666666</v>
+      </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -3286,8 +4375,12 @@
         <f t="shared" si="0"/>
         <v>92.446579304854851</v>
       </c>
+      <c r="N15">
+        <f t="shared" si="1"/>
+        <v>-175.83440000000002</v>
+      </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -3328,8 +4421,12 @@
         <f t="shared" si="0"/>
         <v>61.421707887226404</v>
       </c>
+      <c r="N16">
+        <f t="shared" si="1"/>
+        <v>-179.46962133333329</v>
+      </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -3370,8 +4467,12 @@
         <f t="shared" si="0"/>
         <v>-85.26801343285581</v>
       </c>
+      <c r="N17">
+        <f t="shared" si="1"/>
+        <v>-13.053684000000032</v>
+      </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -3412,8 +4513,12 @@
         <f t="shared" si="0"/>
         <v>-100.47202834386164</v>
       </c>
+      <c r="N18">
+        <f t="shared" si="1"/>
+        <v>-34.96407233333332</v>
+      </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -3454,8 +4559,12 @@
         <f t="shared" si="0"/>
         <v>-118.55614392917474</v>
       </c>
+      <c r="N19">
+        <f t="shared" si="1"/>
+        <v>-65.23229166666664</v>
+      </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -3496,8 +4605,12 @@
         <f t="shared" si="0"/>
         <v>-130.34534471494399</v>
       </c>
+      <c r="N20">
+        <f t="shared" si="1"/>
+        <v>-62.34820133333335</v>
+      </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -3538,8 +4651,12 @@
         <f t="shared" si="0"/>
         <v>-176.45805249972761</v>
       </c>
+      <c r="N21">
+        <f t="shared" si="1"/>
+        <v>-117.29189900000006</v>
+      </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -3580,8 +4697,12 @@
         <f t="shared" si="0"/>
         <v>159.41567628088626</v>
       </c>
+      <c r="N22">
+        <f t="shared" si="1"/>
+        <v>-112.7248013333334</v>
+      </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -3622,8 +4743,12 @@
         <f t="shared" si="0"/>
         <v>126.3871665494629</v>
       </c>
+      <c r="N23">
+        <f t="shared" si="1"/>
+        <v>-143.9102166666666</v>
+      </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -3664,8 +4789,12 @@
         <f t="shared" si="0"/>
         <v>97.117359556282238</v>
       </c>
+      <c r="N24">
+        <f t="shared" si="1"/>
+        <v>-174.45932666666658</v>
+      </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -3706,8 +4835,12 @@
         <f t="shared" si="0"/>
         <v>76.316926612807222</v>
       </c>
+      <c r="N25">
+        <f t="shared" si="1"/>
+        <v>-178.45382600000005</v>
+      </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>12</v>
       </c>
@@ -3748,8 +4881,12 @@
         <f t="shared" si="0"/>
         <v>-19.043530573043078</v>
       </c>
+      <c r="N26">
+        <f t="shared" si="1"/>
+        <v>-37.610962666666637</v>
+      </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -3790,8 +4927,12 @@
         <f t="shared" si="0"/>
         <v>-91.832839505942061</v>
       </c>
+      <c r="N27">
+        <f t="shared" si="1"/>
+        <v>-33.18410833333337</v>
+      </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -3832,8 +4973,12 @@
         <f t="shared" si="0"/>
         <v>-120.44727416607188</v>
       </c>
+      <c r="N28">
+        <f t="shared" si="1"/>
+        <v>-52.248450666666713</v>
+      </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -3874,8 +5019,12 @@
         <f t="shared" si="0"/>
         <v>-128.07612520508755</v>
       </c>
+      <c r="N29">
+        <f t="shared" si="1"/>
+        <v>-60.876977333333343</v>
+      </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -3916,8 +5065,12 @@
         <f t="shared" si="0"/>
         <v>-166.57456259797561</v>
       </c>
+      <c r="N30">
+        <f t="shared" si="1"/>
+        <v>-112.11438899999996</v>
+      </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>12</v>
       </c>
@@ -3958,8 +5111,12 @@
         <f t="shared" si="0"/>
         <v>156.20412753612658</v>
       </c>
+      <c r="N31">
+        <f t="shared" si="1"/>
+        <v>-119.75794833333339</v>
+      </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>12</v>
       </c>
@@ -4000,8 +5157,12 @@
         <f t="shared" si="0"/>
         <v>137.34434478917723</v>
       </c>
+      <c r="N32">
+        <f t="shared" si="1"/>
+        <v>-159.69576833333338</v>
+      </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>12</v>
       </c>
@@ -4042,8 +5203,12 @@
         <f t="shared" si="0"/>
         <v>101.70584311045958</v>
       </c>
+      <c r="N33">
+        <f t="shared" si="1"/>
+        <v>-157.83128866666664</v>
+      </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>12</v>
       </c>
@@ -4084,8 +5249,12 @@
         <f t="shared" si="0"/>
         <v>80.965642501176617</v>
       </c>
+      <c r="N34">
+        <f t="shared" si="1"/>
+        <v>-156.43324000000007</v>
+      </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>12</v>
       </c>
@@ -4126,8 +5295,12 @@
         <f t="shared" si="0"/>
         <v>-6.444113843882759</v>
       </c>
+      <c r="N35">
+        <f t="shared" si="1"/>
+        <v>-10.384231333333332</v>
+      </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>12</v>
       </c>
@@ -4168,8 +5341,12 @@
         <f t="shared" si="0"/>
         <v>-95.877915989604176</v>
       </c>
+      <c r="N36">
+        <f t="shared" si="1"/>
+        <v>-21.489542000000029</v>
+      </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>12</v>
       </c>
@@ -4210,8 +5387,12 @@
         <f t="shared" si="0"/>
         <v>-113.57778614409671</v>
       </c>
+      <c r="N37">
+        <f t="shared" si="1"/>
+        <v>-37.978282999999919</v>
+      </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>12</v>
       </c>
@@ -4252,8 +5433,12 @@
         <f t="shared" si="0"/>
         <v>-120.31625911789547</v>
       </c>
+      <c r="N38">
+        <f t="shared" si="1"/>
+        <v>-78.791965333333565</v>
+      </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>12</v>
       </c>
@@ -4294,8 +5479,12 @@
         <f t="shared" si="0"/>
         <v>-155.46469684426029</v>
       </c>
+      <c r="N39">
+        <f t="shared" si="1"/>
+        <v>-75.683770666666646</v>
+      </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>12</v>
       </c>
@@ -4336,8 +5525,12 @@
         <f t="shared" si="0"/>
         <v>168.75556199757222</v>
       </c>
+      <c r="N40">
+        <f t="shared" si="1"/>
+        <v>-86.477631999999971</v>
+      </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>12</v>
       </c>
@@ -4378,8 +5571,12 @@
         <f t="shared" si="0"/>
         <v>134.94406531599958</v>
       </c>
+      <c r="N41">
+        <f t="shared" si="1"/>
+        <v>-151.63612933333332</v>
+      </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>12</v>
       </c>
@@ -4420,8 +5617,12 @@
         <f t="shared" si="0"/>
         <v>108.46181041472478</v>
       </c>
+      <c r="N42">
+        <f t="shared" si="1"/>
+        <v>-2.0269263333333356</v>
+      </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>12</v>
       </c>
@@ -4462,8 +5663,12 @@
         <f t="shared" si="0"/>
         <v>82.741783783704264</v>
       </c>
+      <c r="N43">
+        <f t="shared" si="1"/>
+        <v>-5.693752666666569</v>
+      </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>12</v>
       </c>
@@ -4504,8 +5709,12 @@
         <f t="shared" si="0"/>
         <v>18.904575842611656</v>
       </c>
+      <c r="N44">
+        <f t="shared" si="1"/>
+        <v>-45.392747666666651</v>
+      </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>12</v>
       </c>
@@ -4546,8 +5755,12 @@
         <f t="shared" si="0"/>
         <v>-92.682823844806236</v>
       </c>
+      <c r="N45">
+        <f t="shared" si="1"/>
+        <v>-23.403636666666671</v>
+      </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>12</v>
       </c>
@@ -4588,8 +5801,12 @@
         <f t="shared" si="0"/>
         <v>-108.90386410263935</v>
       </c>
+      <c r="N46">
+        <f t="shared" si="1"/>
+        <v>-9.6548303333332797</v>
+      </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>12</v>
       </c>
@@ -4630,8 +5847,12 @@
         <f t="shared" si="0"/>
         <v>-122.77038424244212</v>
       </c>
+      <c r="N47">
+        <f t="shared" si="1"/>
+        <v>-44.295946000000072</v>
+      </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>12</v>
       </c>
@@ -4672,8 +5893,12 @@
         <f t="shared" si="0"/>
         <v>-154.26651085419394</v>
       </c>
+      <c r="N48">
+        <f t="shared" si="1"/>
+        <v>-108.63577000000009</v>
+      </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>12</v>
       </c>
@@ -4714,8 +5939,12 @@
         <f t="shared" si="0"/>
         <v>172.94301739649899</v>
       </c>
+      <c r="N49">
+        <f t="shared" si="1"/>
+        <v>-122.09115399999996</v>
+      </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>12</v>
       </c>
@@ -4756,8 +5985,12 @@
         <f t="shared" si="0"/>
         <v>143.30538742507804</v>
       </c>
+      <c r="N50">
+        <f t="shared" si="1"/>
+        <v>-160.21116799999982</v>
+      </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>12</v>
       </c>
@@ -4798,8 +6031,12 @@
         <f t="shared" si="0"/>
         <v>122.61182966061835</v>
       </c>
+      <c r="N51">
+        <f t="shared" si="1"/>
+        <v>-134.28737999999998</v>
+      </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>12</v>
       </c>
@@ -4840,8 +6077,12 @@
         <f t="shared" si="0"/>
         <v>87.540392604636423</v>
       </c>
+      <c r="N52">
+        <f t="shared" si="1"/>
+        <v>-30.889729999999872</v>
+      </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>12</v>
       </c>
@@ -4882,8 +6123,12 @@
         <f t="shared" si="0"/>
         <v>34.418364479056208</v>
       </c>
+      <c r="N53">
+        <f t="shared" si="1"/>
+        <v>-13.044759999999997</v>
+      </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>12</v>
       </c>
@@ -4924,8 +6169,12 @@
         <f t="shared" si="0"/>
         <v>-73.545371985980367</v>
       </c>
+      <c r="N54">
+        <f t="shared" si="1"/>
+        <v>-75.724416666666684</v>
+      </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>12</v>
       </c>
@@ -4966,8 +6215,12 @@
         <f t="shared" si="0"/>
         <v>-103.70161120260745</v>
       </c>
+      <c r="N55">
+        <f t="shared" si="1"/>
+        <v>-40.208918666666705</v>
+      </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>12</v>
       </c>
@@ -5008,8 +6261,12 @@
         <f t="shared" si="0"/>
         <v>-120.27431923344497</v>
       </c>
+      <c r="N56">
+        <f t="shared" si="1"/>
+        <v>-33.948999000000185</v>
+      </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>12</v>
       </c>
@@ -5050,8 +6307,12 @@
         <f t="shared" si="0"/>
         <v>-144.16903110769712</v>
       </c>
+      <c r="N57">
+        <f t="shared" si="1"/>
+        <v>-51.951333333333324</v>
+      </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>12</v>
       </c>

</xml_diff>